<commit_message>
-- Continued adding BOM parts -- Removed Current Sense filtering
</commit_message>
<xml_diff>
--- a/DOCS/BOM/bldc_driver_board.xlsx
+++ b/DOCS/BOM/bldc_driver_board.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A93A181-075B-4B52-A28D-D625B8E23E15}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52774DD3-7A81-41CA-A28A-C6DC2EBA6F2E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
   <si>
     <t>Referenz</t>
   </si>
@@ -76,9 +76,6 @@
     <t>10 uF, 16 V Elko</t>
   </si>
   <si>
-    <t>C12, C15, C18</t>
-  </si>
-  <si>
     <t>1uF, 6.3V Capacitor</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>1 uF, 16 V Capacitor</t>
   </si>
   <si>
-    <t>2200 pF, 6,3 V Capacitor</t>
-  </si>
-  <si>
     <t>10 pF, 25 V Capacitor</t>
   </si>
   <si>
@@ -158,6 +152,48 @@
   </si>
   <si>
     <t>R5</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>169k Resister</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>9.31k Resistor</t>
+  </si>
+  <si>
+    <t>R11, R12, R13</t>
+  </si>
+  <si>
+    <t>1k Resistor</t>
+  </si>
+  <si>
+    <t>R17, R18, R19</t>
+  </si>
+  <si>
+    <t>0.002 Resistor</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>HTQPF-48</t>
+  </si>
+  <si>
+    <t>BLDC Gate Driver IC</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOIC-8 </t>
+  </si>
+  <si>
+    <t>CAN Transceiver</t>
   </si>
 </sst>
 </file>
@@ -220,12 +256,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -507,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,288 +565,373 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="3">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="3">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="3">
+        <v>6</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="4">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="E16" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="3">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="3">
+        <v>3</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4">
-        <v>2</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="4">
-        <v>3</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="4">
-        <v>3</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="4">
-        <v>1</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="4">
-        <v>3</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="4">
-        <v>3</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="4">
-        <v>2</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="4">
-        <v>6</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="4">
-        <v>1</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="6" t="s">
+      <c r="D20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -825,19 +946,24 @@
     <hyperlink ref="E6" r:id="rId4" xr:uid="{91FF59B1-021D-470D-8639-0E4C9D34C9F1}"/>
     <hyperlink ref="E7" r:id="rId5" xr:uid="{320CA672-E678-4BF1-AF9C-FF2AFA78BFB8}"/>
     <hyperlink ref="E8" r:id="rId6" xr:uid="{23D1F2CB-CA76-40FE-9394-B2CFD7E95EF9}"/>
-    <hyperlink ref="E9" r:id="rId7" xr:uid="{FE0F1438-2C62-4E7F-B6C3-6715A279E86A}"/>
-    <hyperlink ref="E10" r:id="rId8" xr:uid="{A4C09D8C-77DF-4AEE-ADE6-7C3575037047}"/>
-    <hyperlink ref="E11" r:id="rId9" xr:uid="{2B079660-BC8B-4D6C-87DE-C93CFC7622E6}"/>
-    <hyperlink ref="E13" r:id="rId10" xr:uid="{14D46A7F-E0A6-406B-A7EE-289B3FAD4FBF}"/>
-    <hyperlink ref="E14" r:id="rId11" xr:uid="{5327B70B-4C91-4436-8F09-0558C954814C}"/>
-    <hyperlink ref="E15" r:id="rId12" xr:uid="{26EB56AD-70D4-45FC-A02C-69F313B73A86}"/>
-    <hyperlink ref="F15" r:id="rId13" xr:uid="{F6178EC9-4068-46A9-9686-3B2D776C9F8A}"/>
-    <hyperlink ref="E2" r:id="rId14" xr:uid="{5C7B406A-1DBE-4F13-B09B-357D8FF3969B}"/>
-    <hyperlink ref="E12" r:id="rId15" xr:uid="{6DB27604-3813-4A10-B108-70406FEAA52E}"/>
-    <hyperlink ref="E16" r:id="rId16" xr:uid="{943E92B4-D842-4139-918E-0BEB544D3EF9}"/>
-    <hyperlink ref="E17" r:id="rId17" xr:uid="{A2B967F3-32C5-4942-935C-B061F0744102}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{A4C09D8C-77DF-4AEE-ADE6-7C3575037047}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{2B079660-BC8B-4D6C-87DE-C93CFC7622E6}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{14D46A7F-E0A6-406B-A7EE-289B3FAD4FBF}"/>
+    <hyperlink ref="E13" r:id="rId10" xr:uid="{5327B70B-4C91-4436-8F09-0558C954814C}"/>
+    <hyperlink ref="E14" r:id="rId11" xr:uid="{26EB56AD-70D4-45FC-A02C-69F313B73A86}"/>
+    <hyperlink ref="F14" r:id="rId12" xr:uid="{F6178EC9-4068-46A9-9686-3B2D776C9F8A}"/>
+    <hyperlink ref="E2" r:id="rId13" xr:uid="{5C7B406A-1DBE-4F13-B09B-357D8FF3969B}"/>
+    <hyperlink ref="E11" r:id="rId14" xr:uid="{6DB27604-3813-4A10-B108-70406FEAA52E}"/>
+    <hyperlink ref="E15" r:id="rId15" xr:uid="{943E92B4-D842-4139-918E-0BEB544D3EF9}"/>
+    <hyperlink ref="E16" r:id="rId16" xr:uid="{A2B967F3-32C5-4942-935C-B061F0744102}"/>
+    <hyperlink ref="E17" r:id="rId17" xr:uid="{F12099C4-E221-44DB-BDDE-75EFA49EE8A2}"/>
+    <hyperlink ref="E18" r:id="rId18" xr:uid="{0870E44A-54FA-46F5-AD38-36FF7650324A}"/>
+    <hyperlink ref="E19" r:id="rId19" xr:uid="{AA67CB40-C2C9-4916-96BF-96FB528240DE}"/>
+    <hyperlink ref="E20" r:id="rId20" xr:uid="{A79AE12B-A5F7-47C1-A554-4DB9AF312B4B}"/>
+    <hyperlink ref="E21" r:id="rId21" xr:uid="{B7756788-37D9-43AE-857C-EE73ABC40F38}"/>
+    <hyperlink ref="E22" r:id="rId22" xr:uid="{DD1A5CC6-ED82-4F13-9985-BC75FFA6CAB1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-- Modified part list
</commit_message>
<xml_diff>
--- a/DOCS/BOM/bldc_driver_board.xlsx
+++ b/DOCS/BOM/bldc_driver_board.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52774DD3-7A81-41CA-A28A-C6DC2EBA6F2E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA3F252-05F8-4440-A1AC-18B6D1CF3FAE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="28800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
     <t>Referenz</t>
   </si>
@@ -109,12 +109,6 @@
     <t>C20, C21, C22</t>
   </si>
   <si>
-    <t>220 nF, 100 V Capacitor</t>
-  </si>
-  <si>
-    <t>C23, C24, C25</t>
-  </si>
-  <si>
     <t>BAT30KFILM Diode</t>
   </si>
   <si>
@@ -194,6 +188,9 @@
   </si>
   <si>
     <t>CAN Transceiver</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -543,21 +540,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
     <col min="2" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.7265625" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -565,7 +562,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -575,7 +572,7 @@
       </c>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -591,8 +588,11 @@
       <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -608,8 +608,11 @@
       <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -625,8 +628,11 @@
       <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -642,8 +648,11 @@
       <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -659,8 +668,11 @@
       <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -676,8 +688,11 @@
       <c r="E7" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -693,8 +708,11 @@
       <c r="E8" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -710,8 +728,11 @@
       <c r="E9" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
@@ -727,8 +748,11 @@
       <c r="E10" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
@@ -739,21 +763,24 @@
         <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B12" s="3">
-        <v>3</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>29</v>
@@ -761,64 +788,73 @@
       <c r="E12" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="G12" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="3">
-        <v>2</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="E13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="3">
+        <v>6</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B14">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B15" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -827,13 +863,16 @@
         <v>8</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>44</v>
       </c>
@@ -849,13 +888,16 @@
       <c r="E17" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B18" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>8</v>
@@ -866,8 +908,11 @@
       <c r="E18" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>48</v>
       </c>
@@ -875,7 +920,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>49</v>
@@ -883,56 +928,48 @@
       <c r="E19" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B20" s="3">
-        <v>3</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G20" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B21" s="3">
         <v>1</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>53</v>
+      <c r="C21" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="3">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>5</v>
+      <c r="G21" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -948,22 +985,21 @@
     <hyperlink ref="E8" r:id="rId6" xr:uid="{23D1F2CB-CA76-40FE-9394-B2CFD7E95EF9}"/>
     <hyperlink ref="E9" r:id="rId7" xr:uid="{A4C09D8C-77DF-4AEE-ADE6-7C3575037047}"/>
     <hyperlink ref="E10" r:id="rId8" xr:uid="{2B079660-BC8B-4D6C-87DE-C93CFC7622E6}"/>
-    <hyperlink ref="E12" r:id="rId9" xr:uid="{14D46A7F-E0A6-406B-A7EE-289B3FAD4FBF}"/>
-    <hyperlink ref="E13" r:id="rId10" xr:uid="{5327B70B-4C91-4436-8F09-0558C954814C}"/>
-    <hyperlink ref="E14" r:id="rId11" xr:uid="{26EB56AD-70D4-45FC-A02C-69F313B73A86}"/>
-    <hyperlink ref="F14" r:id="rId12" xr:uid="{F6178EC9-4068-46A9-9686-3B2D776C9F8A}"/>
-    <hyperlink ref="E2" r:id="rId13" xr:uid="{5C7B406A-1DBE-4F13-B09B-357D8FF3969B}"/>
-    <hyperlink ref="E11" r:id="rId14" xr:uid="{6DB27604-3813-4A10-B108-70406FEAA52E}"/>
-    <hyperlink ref="E15" r:id="rId15" xr:uid="{943E92B4-D842-4139-918E-0BEB544D3EF9}"/>
-    <hyperlink ref="E16" r:id="rId16" xr:uid="{A2B967F3-32C5-4942-935C-B061F0744102}"/>
-    <hyperlink ref="E17" r:id="rId17" xr:uid="{F12099C4-E221-44DB-BDDE-75EFA49EE8A2}"/>
-    <hyperlink ref="E18" r:id="rId18" xr:uid="{0870E44A-54FA-46F5-AD38-36FF7650324A}"/>
-    <hyperlink ref="E19" r:id="rId19" xr:uid="{AA67CB40-C2C9-4916-96BF-96FB528240DE}"/>
-    <hyperlink ref="E20" r:id="rId20" xr:uid="{A79AE12B-A5F7-47C1-A554-4DB9AF312B4B}"/>
-    <hyperlink ref="E21" r:id="rId21" xr:uid="{B7756788-37D9-43AE-857C-EE73ABC40F38}"/>
-    <hyperlink ref="E22" r:id="rId22" xr:uid="{DD1A5CC6-ED82-4F13-9985-BC75FFA6CAB1}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{5327B70B-4C91-4436-8F09-0558C954814C}"/>
+    <hyperlink ref="E13" r:id="rId10" xr:uid="{26EB56AD-70D4-45FC-A02C-69F313B73A86}"/>
+    <hyperlink ref="F13" r:id="rId11" xr:uid="{F6178EC9-4068-46A9-9686-3B2D776C9F8A}"/>
+    <hyperlink ref="E2" r:id="rId12" xr:uid="{5C7B406A-1DBE-4F13-B09B-357D8FF3969B}"/>
+    <hyperlink ref="E11" r:id="rId13" xr:uid="{6DB27604-3813-4A10-B108-70406FEAA52E}"/>
+    <hyperlink ref="E14" r:id="rId14" xr:uid="{943E92B4-D842-4139-918E-0BEB544D3EF9}"/>
+    <hyperlink ref="E15" r:id="rId15" xr:uid="{A2B967F3-32C5-4942-935C-B061F0744102}"/>
+    <hyperlink ref="E16" r:id="rId16" xr:uid="{F12099C4-E221-44DB-BDDE-75EFA49EE8A2}"/>
+    <hyperlink ref="E17" r:id="rId17" xr:uid="{0870E44A-54FA-46F5-AD38-36FF7650324A}"/>
+    <hyperlink ref="E18" r:id="rId18" xr:uid="{AA67CB40-C2C9-4916-96BF-96FB528240DE}"/>
+    <hyperlink ref="E19" r:id="rId19" xr:uid="{A79AE12B-A5F7-47C1-A554-4DB9AF312B4B}"/>
+    <hyperlink ref="E20" r:id="rId20" xr:uid="{B7756788-37D9-43AE-857C-EE73ABC40F38}"/>
+    <hyperlink ref="E21" r:id="rId21" xr:uid="{DD1A5CC6-ED82-4F13-9985-BC75FFA6CAB1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-- Added connectors to partlist
</commit_message>
<xml_diff>
--- a/DOCS/BOM/bldc_driver_board.xlsx
+++ b/DOCS/BOM/bldc_driver_board.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA3F252-05F8-4440-A1AC-18B6D1CF3FAE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE4031D-82F9-4873-8C60-EC7B8801A0F4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="28800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
   <si>
     <t>Referenz</t>
   </si>
@@ -191,6 +191,45 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>2x19 RM2.54</t>
+  </si>
+  <si>
+    <t>Buchsenleiste</t>
+  </si>
+  <si>
+    <t>Conrad</t>
+  </si>
+  <si>
+    <t>J6, J7</t>
+  </si>
+  <si>
+    <t>J2, J3</t>
+  </si>
+  <si>
+    <t>RJ45</t>
+  </si>
+  <si>
+    <t>RJ45 Buchse</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>1x8 RM5.08</t>
+  </si>
+  <si>
+    <t>Motor-Connector</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>1x3 RM5.08</t>
+  </si>
+  <si>
+    <t>PWR-Connector</t>
   </si>
 </sst>
 </file>
@@ -222,7 +261,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,6 +271,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -249,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -259,6 +304,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -540,21 +586,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="28.7265625" customWidth="1"/>
-    <col min="5" max="5" width="10.7265625" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -572,7 +618,7 @@
       </c>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -588,11 +634,11 @@
       <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G2" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -608,11 +654,11 @@
       <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G3" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -628,11 +674,11 @@
       <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G4" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -648,11 +694,11 @@
       <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G5" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -668,11 +714,11 @@
       <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G6" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -688,11 +734,11 @@
       <c r="E7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G7" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -708,11 +754,11 @@
       <c r="E8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G8" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -728,11 +774,11 @@
       <c r="E9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G9" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
@@ -748,11 +794,11 @@
       <c r="E10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G10" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
@@ -768,11 +814,11 @@
       <c r="E11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G11" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
@@ -788,11 +834,11 @@
       <c r="E12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G12" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -811,8 +857,9 @@
       <c r="F13" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
@@ -828,11 +875,11 @@
       <c r="E14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G14" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>41</v>
       </c>
@@ -848,11 +895,11 @@
       <c r="E15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G15" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
@@ -868,11 +915,11 @@
       <c r="E16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G16" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>44</v>
       </c>
@@ -888,11 +935,11 @@
       <c r="E17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G17" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>46</v>
       </c>
@@ -908,11 +955,11 @@
       <c r="E18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G18" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>48</v>
       </c>
@@ -928,11 +975,11 @@
       <c r="E19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G19" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>50</v>
       </c>
@@ -948,11 +995,11 @@
       <c r="E20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G20" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>53</v>
       </c>
@@ -968,7 +1015,87 @@
       <c r="E21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="3">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="3">
+        <v>2</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>56</v>
       </c>
     </row>
@@ -998,8 +1125,12 @@
     <hyperlink ref="E19" r:id="rId19" xr:uid="{A79AE12B-A5F7-47C1-A554-4DB9AF312B4B}"/>
     <hyperlink ref="E20" r:id="rId20" xr:uid="{B7756788-37D9-43AE-857C-EE73ABC40F38}"/>
     <hyperlink ref="E21" r:id="rId21" xr:uid="{DD1A5CC6-ED82-4F13-9985-BC75FFA6CAB1}"/>
+    <hyperlink ref="E22" r:id="rId22" xr:uid="{5D19AACA-AF75-4C83-BF03-58C2CCA870AE}"/>
+    <hyperlink ref="E23" r:id="rId23" xr:uid="{5FABD2FD-90E5-4F9D-826D-19FD52302054}"/>
+    <hyperlink ref="E24" r:id="rId24" xr:uid="{C23E9437-BF03-4016-A0A3-5C72335AAAF4}"/>
+    <hyperlink ref="E25" r:id="rId25" xr:uid="{4B1396C4-03DE-4D44-9AFA-0226DF51047D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-- Added comment due to forgotton resistory
</commit_message>
<xml_diff>
--- a/DOCS/BOM/bldc_driver_board.xlsx
+++ b/DOCS/BOM/bldc_driver_board.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE4031D-82F9-4873-8C60-EC7B8801A0F4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE494D2-B3EB-4170-A8FA-7E4E6B1F1AC5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="71">
   <si>
     <t>Referenz</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>PWR-Connector</t>
+  </si>
+  <si>
+    <t>R4</t>
   </si>
 </sst>
 </file>
@@ -261,7 +264,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,6 +283,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -294,17 +303,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -586,21 +598,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="A15" sqref="A15:G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
     <col min="2" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.7265625" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -613,12 +628,12 @@
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -634,11 +649,11 @@
       <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -654,11 +669,11 @@
       <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -674,11 +689,11 @@
       <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -694,11 +709,11 @@
       <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -714,11 +729,11 @@
       <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -734,11 +749,11 @@
       <c r="E7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -754,11 +769,11 @@
       <c r="E8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -774,11 +789,11 @@
       <c r="E9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
@@ -794,11 +809,11 @@
       <c r="E10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
@@ -814,11 +829,11 @@
       <c r="E11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
@@ -834,11 +849,11 @@
       <c r="E12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -857,9 +872,9 @@
       <c r="F13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
@@ -875,33 +890,24 @@
       <c r="E14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="G14" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B15" s="3">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -910,18 +916,18 @@
         <v>8</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -930,172 +936,192 @@
         <v>8</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" s="3">
         <v>3</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="3">
+        <v>3</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="E20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="3">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="E21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="3">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="E22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B22" s="3">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="B23" s="3">
         <v>2</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B24" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G24" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B25" s="3">
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1118,19 +1144,19 @@
     <hyperlink ref="E2" r:id="rId12" xr:uid="{5C7B406A-1DBE-4F13-B09B-357D8FF3969B}"/>
     <hyperlink ref="E11" r:id="rId13" xr:uid="{6DB27604-3813-4A10-B108-70406FEAA52E}"/>
     <hyperlink ref="E14" r:id="rId14" xr:uid="{943E92B4-D842-4139-918E-0BEB544D3EF9}"/>
-    <hyperlink ref="E15" r:id="rId15" xr:uid="{A2B967F3-32C5-4942-935C-B061F0744102}"/>
-    <hyperlink ref="E16" r:id="rId16" xr:uid="{F12099C4-E221-44DB-BDDE-75EFA49EE8A2}"/>
-    <hyperlink ref="E17" r:id="rId17" xr:uid="{0870E44A-54FA-46F5-AD38-36FF7650324A}"/>
-    <hyperlink ref="E18" r:id="rId18" xr:uid="{AA67CB40-C2C9-4916-96BF-96FB528240DE}"/>
-    <hyperlink ref="E19" r:id="rId19" xr:uid="{A79AE12B-A5F7-47C1-A554-4DB9AF312B4B}"/>
-    <hyperlink ref="E20" r:id="rId20" xr:uid="{B7756788-37D9-43AE-857C-EE73ABC40F38}"/>
-    <hyperlink ref="E21" r:id="rId21" xr:uid="{DD1A5CC6-ED82-4F13-9985-BC75FFA6CAB1}"/>
-    <hyperlink ref="E22" r:id="rId22" xr:uid="{5D19AACA-AF75-4C83-BF03-58C2CCA870AE}"/>
-    <hyperlink ref="E23" r:id="rId23" xr:uid="{5FABD2FD-90E5-4F9D-826D-19FD52302054}"/>
-    <hyperlink ref="E24" r:id="rId24" xr:uid="{C23E9437-BF03-4016-A0A3-5C72335AAAF4}"/>
-    <hyperlink ref="E25" r:id="rId25" xr:uid="{4B1396C4-03DE-4D44-9AFA-0226DF51047D}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{A2B967F3-32C5-4942-935C-B061F0744102}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{F12099C4-E221-44DB-BDDE-75EFA49EE8A2}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{0870E44A-54FA-46F5-AD38-36FF7650324A}"/>
+    <hyperlink ref="E19" r:id="rId18" xr:uid="{AA67CB40-C2C9-4916-96BF-96FB528240DE}"/>
+    <hyperlink ref="E20" r:id="rId19" xr:uid="{A79AE12B-A5F7-47C1-A554-4DB9AF312B4B}"/>
+    <hyperlink ref="E21" r:id="rId20" xr:uid="{B7756788-37D9-43AE-857C-EE73ABC40F38}"/>
+    <hyperlink ref="E22" r:id="rId21" xr:uid="{DD1A5CC6-ED82-4F13-9985-BC75FFA6CAB1}"/>
+    <hyperlink ref="E23" r:id="rId22" xr:uid="{5D19AACA-AF75-4C83-BF03-58C2CCA870AE}"/>
+    <hyperlink ref="E24" r:id="rId23" xr:uid="{5FABD2FD-90E5-4F9D-826D-19FD52302054}"/>
+    <hyperlink ref="E25" r:id="rId24" xr:uid="{C23E9437-BF03-4016-A0A3-5C72335AAAF4}"/>
+    <hyperlink ref="E26" r:id="rId25" xr:uid="{4B1396C4-03DE-4D44-9AFA-0226DF51047D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId26"/>
+  <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>